<commit_message>
feedback page shows right amount of likes and dislikes
</commit_message>
<xml_diff>
--- a/_static/global/LR.xlsx
+++ b/_static/global/LR.xlsx
@@ -19,345 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Numbers</t>
-  </si>
-  <si>
-    <t>meme101</t>
-  </si>
-  <si>
-    <t>meme102</t>
-  </si>
-  <si>
-    <t>meme103</t>
-  </si>
-  <si>
-    <t>meme104</t>
-  </si>
-  <si>
-    <t>meme105</t>
-  </si>
-  <si>
-    <t>meme106</t>
-  </si>
-  <si>
-    <t>meme107</t>
-  </si>
-  <si>
-    <t>meme108</t>
   </si>
   <si>
     <t>Likes</t>
   </si>
   <si>
     <t>Dislikes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(◕ᴗ◕✿)  </t>
-  </si>
-  <si>
-    <t>meme109</t>
-  </si>
-  <si>
-    <t>meme110</t>
-  </si>
-  <si>
-    <t>meme111</t>
-  </si>
-  <si>
-    <t>meme112</t>
-  </si>
-  <si>
-    <t>meme113</t>
-  </si>
-  <si>
-    <t>meme114</t>
-  </si>
-  <si>
-    <t>meme115</t>
-  </si>
-  <si>
-    <t>meme116</t>
-  </si>
-  <si>
-    <t>meme117</t>
-  </si>
-  <si>
-    <t>meme118</t>
-  </si>
-  <si>
-    <t>meme119</t>
-  </si>
-  <si>
-    <t>meme120</t>
-  </si>
-  <si>
-    <t>meme121</t>
-  </si>
-  <si>
-    <t>meme122</t>
-  </si>
-  <si>
-    <t>meme123</t>
-  </si>
-  <si>
-    <t>meme124</t>
-  </si>
-  <si>
-    <t>meme125</t>
-  </si>
-  <si>
-    <t>meme126</t>
-  </si>
-  <si>
-    <t>meme127</t>
-  </si>
-  <si>
-    <t>meme128</t>
-  </si>
-  <si>
-    <t>meme129</t>
-  </si>
-  <si>
-    <t>meme130</t>
-  </si>
-  <si>
-    <t>meme131</t>
-  </si>
-  <si>
-    <t>meme132</t>
-  </si>
-  <si>
-    <t>meme133</t>
-  </si>
-  <si>
-    <t>meme134</t>
-  </si>
-  <si>
-    <t>meme135</t>
-  </si>
-  <si>
-    <t>meme136</t>
-  </si>
-  <si>
-    <t>meme137</t>
-  </si>
-  <si>
-    <t>meme138</t>
-  </si>
-  <si>
-    <t>meme139</t>
-  </si>
-  <si>
-    <t>meme140</t>
-  </si>
-  <si>
-    <t>meme141</t>
-  </si>
-  <si>
-    <t>meme142</t>
-  </si>
-  <si>
-    <t>meme143</t>
-  </si>
-  <si>
-    <t>meme144</t>
-  </si>
-  <si>
-    <t>meme145</t>
-  </si>
-  <si>
-    <t>meme146</t>
-  </si>
-  <si>
-    <t>meme147</t>
-  </si>
-  <si>
-    <t>meme148</t>
-  </si>
-  <si>
-    <t>meme149</t>
-  </si>
-  <si>
-    <t>meme150</t>
-  </si>
-  <si>
-    <t>meme151</t>
-  </si>
-  <si>
-    <t>meme152</t>
-  </si>
-  <si>
-    <t>meme153</t>
-  </si>
-  <si>
-    <t>meme154</t>
-  </si>
-  <si>
-    <t>meme155</t>
-  </si>
-  <si>
-    <t>meme156</t>
-  </si>
-  <si>
-    <t>meme157</t>
-  </si>
-  <si>
-    <t>meme158</t>
-  </si>
-  <si>
-    <t>meme159</t>
-  </si>
-  <si>
-    <t>meme160</t>
-  </si>
-  <si>
-    <t>meme161</t>
-  </si>
-  <si>
-    <t>meme162</t>
-  </si>
-  <si>
-    <t>meme163</t>
-  </si>
-  <si>
-    <t>meme164</t>
-  </si>
-  <si>
-    <t>meme165</t>
-  </si>
-  <si>
-    <t>meme166</t>
-  </si>
-  <si>
-    <t>meme167</t>
-  </si>
-  <si>
-    <t>meme168</t>
-  </si>
-  <si>
-    <t>meme169</t>
-  </si>
-  <si>
-    <t>meme170</t>
-  </si>
-  <si>
-    <t>meme171</t>
-  </si>
-  <si>
-    <t>meme172</t>
-  </si>
-  <si>
-    <t>meme173</t>
-  </si>
-  <si>
-    <t>meme174</t>
-  </si>
-  <si>
-    <t>meme175</t>
-  </si>
-  <si>
-    <t>meme176</t>
-  </si>
-  <si>
-    <t>meme177</t>
-  </si>
-  <si>
-    <t>meme178</t>
-  </si>
-  <si>
-    <t>meme179</t>
-  </si>
-  <si>
-    <t>meme180</t>
-  </si>
-  <si>
-    <t>meme181</t>
-  </si>
-  <si>
-    <t>meme182</t>
-  </si>
-  <si>
-    <t>meme183</t>
-  </si>
-  <si>
-    <t>meme184</t>
-  </si>
-  <si>
-    <t>meme185</t>
-  </si>
-  <si>
-    <t>meme186</t>
-  </si>
-  <si>
-    <t>meme187</t>
-  </si>
-  <si>
-    <t>meme188</t>
-  </si>
-  <si>
-    <t>meme189</t>
-  </si>
-  <si>
-    <t>meme190</t>
-  </si>
-  <si>
-    <t>meme191</t>
-  </si>
-  <si>
-    <t>meme192</t>
-  </si>
-  <si>
-    <t>meme193</t>
-  </si>
-  <si>
-    <t>meme194</t>
-  </si>
-  <si>
-    <t>meme195</t>
-  </si>
-  <si>
-    <t>meme196</t>
-  </si>
-  <si>
-    <t>meme197</t>
-  </si>
-  <si>
-    <t>meme198</t>
-  </si>
-  <si>
-    <t>meme199</t>
-  </si>
-  <si>
-    <t>meme200</t>
-  </si>
-  <si>
-    <t>meme201</t>
-  </si>
-  <si>
-    <t>meme202</t>
-  </si>
-  <si>
-    <t>meme203</t>
-  </si>
-  <si>
-    <t>meme204</t>
-  </si>
-  <si>
-    <t>meme205</t>
-  </si>
-  <si>
-    <t>meme206</t>
-  </si>
-  <si>
-    <t>meme207</t>
-  </si>
-  <si>
-    <t>meme208</t>
-  </si>
-  <si>
-    <t>low reward memes</t>
   </si>
 </sst>
 </file>
@@ -741,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -753,26 +423,20 @@
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>101</v>
       </c>
       <c r="B2" s="2">
         <v>20</v>
@@ -781,9 +445,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>102</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
@@ -792,9 +456,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>3</v>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>103</v>
       </c>
       <c r="B4" s="2">
         <v>20</v>
@@ -803,9 +467,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>4</v>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>104</v>
       </c>
       <c r="B5" s="2">
         <v>20</v>
@@ -814,9 +478,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>5</v>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>105</v>
       </c>
       <c r="B6" s="2">
         <v>20</v>
@@ -825,9 +489,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>6</v>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>106</v>
       </c>
       <c r="B7" s="2">
         <v>20</v>
@@ -836,9 +500,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>7</v>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>107</v>
       </c>
       <c r="B8" s="2">
         <v>20</v>
@@ -847,9 +511,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>8</v>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>108</v>
       </c>
       <c r="B9" s="2">
         <v>20</v>
@@ -858,9 +522,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>12</v>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>109</v>
       </c>
       <c r="B10" s="2">
         <v>20</v>
@@ -869,9 +533,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>13</v>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>110</v>
       </c>
       <c r="B11" s="2">
         <v>20</v>
@@ -880,9 +544,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>14</v>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>111</v>
       </c>
       <c r="B12" s="2">
         <v>20</v>
@@ -891,9 +555,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>15</v>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>112</v>
       </c>
       <c r="B13" s="2">
         <v>20</v>
@@ -902,9 +566,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>16</v>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>113</v>
       </c>
       <c r="B14" s="2">
         <v>20</v>
@@ -913,9 +577,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>17</v>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>114</v>
       </c>
       <c r="B15" s="2">
         <v>20</v>
@@ -924,9 +588,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>18</v>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>115</v>
       </c>
       <c r="B16" s="2">
         <v>20</v>
@@ -936,8 +600,8 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>19</v>
+      <c r="A17">
+        <v>116</v>
       </c>
       <c r="B17" s="2">
         <v>20</v>
@@ -947,8 +611,8 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>20</v>
+      <c r="A18">
+        <v>117</v>
       </c>
       <c r="B18" s="2">
         <v>20</v>
@@ -958,8 +622,8 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>21</v>
+      <c r="A19">
+        <v>118</v>
       </c>
       <c r="B19" s="2">
         <v>20</v>
@@ -969,8 +633,8 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>22</v>
+      <c r="A20">
+        <v>119</v>
       </c>
       <c r="B20" s="2">
         <v>20</v>
@@ -980,8 +644,8 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>23</v>
+      <c r="A21">
+        <v>120</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
@@ -991,8 +655,8 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>24</v>
+      <c r="A22">
+        <v>121</v>
       </c>
       <c r="B22" s="2">
         <v>19</v>
@@ -1002,8 +666,8 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>25</v>
+      <c r="A23">
+        <v>122</v>
       </c>
       <c r="B23" s="2">
         <v>19</v>
@@ -1013,8 +677,8 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>26</v>
+      <c r="A24">
+        <v>123</v>
       </c>
       <c r="B24" s="2">
         <v>19</v>
@@ -1024,8 +688,8 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>27</v>
+      <c r="A25">
+        <v>124</v>
       </c>
       <c r="B25" s="2">
         <v>19</v>
@@ -1035,8 +699,8 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>28</v>
+      <c r="A26">
+        <v>125</v>
       </c>
       <c r="B26" s="2">
         <v>19</v>
@@ -1046,8 +710,8 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>29</v>
+      <c r="A27">
+        <v>126</v>
       </c>
       <c r="B27" s="2">
         <v>19</v>
@@ -1057,8 +721,8 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>30</v>
+      <c r="A28">
+        <v>127</v>
       </c>
       <c r="B28" s="2">
         <v>17</v>
@@ -1068,8 +732,8 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>31</v>
+      <c r="A29">
+        <v>128</v>
       </c>
       <c r="B29" s="2">
         <v>17</v>
@@ -1079,8 +743,8 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>32</v>
+      <c r="A30">
+        <v>129</v>
       </c>
       <c r="B30" s="2">
         <v>17</v>
@@ -1090,8 +754,8 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>33</v>
+      <c r="A31">
+        <v>130</v>
       </c>
       <c r="B31" s="2">
         <v>17</v>
@@ -1101,8 +765,8 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>34</v>
+      <c r="A32">
+        <v>131</v>
       </c>
       <c r="B32" s="2">
         <v>17</v>
@@ -1112,8 +776,8 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>35</v>
+      <c r="A33">
+        <v>132</v>
       </c>
       <c r="B33" s="2">
         <v>17</v>
@@ -1123,8 +787,8 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>36</v>
+      <c r="A34">
+        <v>133</v>
       </c>
       <c r="B34" s="2">
         <v>17</v>
@@ -1134,8 +798,8 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>37</v>
+      <c r="A35">
+        <v>134</v>
       </c>
       <c r="B35" s="2">
         <v>17</v>
@@ -1145,8 +809,8 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>38</v>
+      <c r="A36">
+        <v>135</v>
       </c>
       <c r="B36" s="2">
         <v>16</v>
@@ -1156,8 +820,8 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>39</v>
+      <c r="A37">
+        <v>136</v>
       </c>
       <c r="B37" s="2">
         <v>16</v>
@@ -1167,8 +831,8 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>40</v>
+      <c r="A38">
+        <v>137</v>
       </c>
       <c r="B38" s="2">
         <v>16</v>
@@ -1178,8 +842,8 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>41</v>
+      <c r="A39">
+        <v>138</v>
       </c>
       <c r="B39" s="2">
         <v>16</v>
@@ -1189,8 +853,8 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>42</v>
+      <c r="A40">
+        <v>139</v>
       </c>
       <c r="B40" s="2">
         <v>16</v>
@@ -1200,8 +864,8 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>43</v>
+      <c r="A41">
+        <v>140</v>
       </c>
       <c r="B41" s="2">
         <v>16</v>
@@ -1211,8 +875,8 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>44</v>
+      <c r="A42">
+        <v>141</v>
       </c>
       <c r="B42" s="2">
         <v>16</v>
@@ -1222,8 +886,8 @@
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>45</v>
+      <c r="A43">
+        <v>142</v>
       </c>
       <c r="B43" s="2">
         <v>16</v>
@@ -1233,8 +897,8 @@
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>46</v>
+      <c r="A44">
+        <v>143</v>
       </c>
       <c r="B44" s="2">
         <v>15</v>
@@ -1244,8 +908,8 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>47</v>
+      <c r="A45">
+        <v>144</v>
       </c>
       <c r="B45" s="2">
         <v>15</v>
@@ -1255,8 +919,8 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>48</v>
+      <c r="A46">
+        <v>145</v>
       </c>
       <c r="B46" s="2">
         <v>15</v>
@@ -1266,8 +930,8 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>49</v>
+      <c r="A47">
+        <v>146</v>
       </c>
       <c r="B47" s="2">
         <v>15</v>
@@ -1277,8 +941,8 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>50</v>
+      <c r="A48">
+        <v>147</v>
       </c>
       <c r="B48" s="2">
         <v>14</v>
@@ -1288,8 +952,8 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>51</v>
+      <c r="A49">
+        <v>148</v>
       </c>
       <c r="B49" s="2">
         <v>14</v>
@@ -1299,8 +963,8 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>52</v>
+      <c r="A50">
+        <v>149</v>
       </c>
       <c r="B50" s="2">
         <v>14</v>
@@ -1310,8 +974,8 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>53</v>
+      <c r="A51">
+        <v>150</v>
       </c>
       <c r="B51" s="2">
         <v>14</v>
@@ -1321,8 +985,8 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>54</v>
+      <c r="A52">
+        <v>151</v>
       </c>
       <c r="B52" s="2">
         <v>14</v>
@@ -1332,8 +996,8 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>55</v>
+      <c r="A53">
+        <v>152</v>
       </c>
       <c r="B53" s="2">
         <v>14</v>
@@ -1343,8 +1007,8 @@
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>56</v>
+      <c r="A54">
+        <v>153</v>
       </c>
       <c r="B54" s="2">
         <v>14</v>
@@ -1354,8 +1018,8 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>57</v>
+      <c r="A55">
+        <v>154</v>
       </c>
       <c r="B55" s="2">
         <v>14</v>
@@ -1365,8 +1029,8 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>58</v>
+      <c r="A56">
+        <v>155</v>
       </c>
       <c r="B56" s="2">
         <v>14</v>
@@ -1376,8 +1040,8 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>59</v>
+      <c r="A57">
+        <v>156</v>
       </c>
       <c r="B57" s="2">
         <v>14</v>
@@ -1387,8 +1051,8 @@
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>60</v>
+      <c r="A58">
+        <v>157</v>
       </c>
       <c r="B58" s="2">
         <v>14</v>
@@ -1398,8 +1062,8 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>61</v>
+      <c r="A59">
+        <v>158</v>
       </c>
       <c r="B59" s="2">
         <v>14</v>
@@ -1409,8 +1073,8 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>62</v>
+      <c r="A60">
+        <v>159</v>
       </c>
       <c r="B60" s="2">
         <v>14</v>
@@ -1420,8 +1084,8 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>63</v>
+      <c r="A61">
+        <v>160</v>
       </c>
       <c r="B61" s="2">
         <v>14</v>
@@ -1431,8 +1095,8 @@
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>64</v>
+      <c r="A62">
+        <v>161</v>
       </c>
       <c r="B62" s="2">
         <v>14</v>
@@ -1442,8 +1106,8 @@
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>65</v>
+      <c r="A63">
+        <v>162</v>
       </c>
       <c r="B63" s="2">
         <v>13</v>
@@ -1453,8 +1117,8 @@
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>66</v>
+      <c r="A64">
+        <v>163</v>
       </c>
       <c r="B64" s="2">
         <v>13</v>
@@ -1464,8 +1128,8 @@
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>67</v>
+      <c r="A65">
+        <v>164</v>
       </c>
       <c r="B65" s="2">
         <v>13</v>
@@ -1475,8 +1139,8 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>68</v>
+      <c r="A66">
+        <v>165</v>
       </c>
       <c r="B66" s="2">
         <v>13</v>
@@ -1486,8 +1150,8 @@
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>69</v>
+      <c r="A67">
+        <v>166</v>
       </c>
       <c r="B67" s="2">
         <v>13</v>
@@ -1497,8 +1161,8 @@
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>70</v>
+      <c r="A68">
+        <v>167</v>
       </c>
       <c r="B68" s="2">
         <v>13</v>
@@ -1508,8 +1172,8 @@
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>71</v>
+      <c r="A69">
+        <v>168</v>
       </c>
       <c r="B69" s="2">
         <v>13</v>
@@ -1519,8 +1183,8 @@
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>72</v>
+      <c r="A70">
+        <v>169</v>
       </c>
       <c r="B70" s="2">
         <v>13</v>
@@ -1530,8 +1194,8 @@
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>73</v>
+      <c r="A71">
+        <v>170</v>
       </c>
       <c r="B71" s="2">
         <v>13</v>
@@ -1541,8 +1205,8 @@
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>74</v>
+      <c r="A72">
+        <v>171</v>
       </c>
       <c r="B72" s="2">
         <v>13</v>
@@ -1552,8 +1216,8 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>75</v>
+      <c r="A73">
+        <v>172</v>
       </c>
       <c r="B73" s="2">
         <v>12</v>
@@ -1563,8 +1227,8 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>76</v>
+      <c r="A74">
+        <v>173</v>
       </c>
       <c r="B74" s="2">
         <v>12</v>
@@ -1574,8 +1238,8 @@
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>77</v>
+      <c r="A75">
+        <v>174</v>
       </c>
       <c r="B75" s="2">
         <v>12</v>
@@ -1585,8 +1249,8 @@
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>78</v>
+      <c r="A76">
+        <v>175</v>
       </c>
       <c r="B76" s="2">
         <v>12</v>
@@ -1596,8 +1260,8 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>79</v>
+      <c r="A77">
+        <v>176</v>
       </c>
       <c r="B77" s="2">
         <v>12</v>
@@ -1607,8 +1271,8 @@
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>80</v>
+      <c r="A78">
+        <v>177</v>
       </c>
       <c r="B78" s="2">
         <v>12</v>
@@ -1618,8 +1282,8 @@
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>81</v>
+      <c r="A79">
+        <v>178</v>
       </c>
       <c r="B79" s="2">
         <v>12</v>
@@ -1629,8 +1293,8 @@
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>82</v>
+      <c r="A80">
+        <v>179</v>
       </c>
       <c r="B80" s="2">
         <v>12</v>
@@ -1640,8 +1304,8 @@
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>83</v>
+      <c r="A81">
+        <v>180</v>
       </c>
       <c r="B81" s="2">
         <v>11</v>
@@ -1651,8 +1315,8 @@
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>84</v>
+      <c r="A82">
+        <v>181</v>
       </c>
       <c r="B82" s="2">
         <v>11</v>
@@ -1662,8 +1326,8 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>85</v>
+      <c r="A83">
+        <v>182</v>
       </c>
       <c r="B83" s="2">
         <v>11</v>
@@ -1673,8 +1337,8 @@
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" t="s">
-        <v>86</v>
+      <c r="A84">
+        <v>183</v>
       </c>
       <c r="B84" s="2">
         <v>11</v>
@@ -1684,8 +1348,8 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" t="s">
-        <v>87</v>
+      <c r="A85">
+        <v>184</v>
       </c>
       <c r="B85" s="2">
         <v>11</v>
@@ -1695,8 +1359,8 @@
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" t="s">
-        <v>88</v>
+      <c r="A86">
+        <v>185</v>
       </c>
       <c r="B86" s="2">
         <v>11</v>
@@ -1706,8 +1370,8 @@
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" t="s">
-        <v>89</v>
+      <c r="A87">
+        <v>186</v>
       </c>
       <c r="B87" s="2">
         <v>11</v>
@@ -1717,8 +1381,8 @@
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>90</v>
+      <c r="A88">
+        <v>187</v>
       </c>
       <c r="B88" s="2">
         <v>11</v>
@@ -1728,8 +1392,8 @@
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" t="s">
-        <v>91</v>
+      <c r="A89">
+        <v>188</v>
       </c>
       <c r="B89" s="2">
         <v>10</v>
@@ -1739,8 +1403,8 @@
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" t="s">
-        <v>92</v>
+      <c r="A90">
+        <v>189</v>
       </c>
       <c r="B90" s="2">
         <v>10</v>
@@ -1750,8 +1414,8 @@
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>93</v>
+      <c r="A91">
+        <v>190</v>
       </c>
       <c r="B91" s="2">
         <v>10</v>
@@ -1761,8 +1425,8 @@
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>94</v>
+      <c r="A92">
+        <v>191</v>
       </c>
       <c r="B92" s="2">
         <v>10</v>
@@ -1772,8 +1436,8 @@
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" t="s">
-        <v>95</v>
+      <c r="A93">
+        <v>192</v>
       </c>
       <c r="B93" s="2">
         <v>10</v>
@@ -1783,8 +1447,8 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>96</v>
+      <c r="A94">
+        <v>193</v>
       </c>
       <c r="B94" s="2">
         <v>10</v>
@@ -1794,8 +1458,8 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>97</v>
+      <c r="A95">
+        <v>194</v>
       </c>
       <c r="B95" s="2">
         <v>10</v>
@@ -1805,8 +1469,8 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" t="s">
-        <v>98</v>
+      <c r="A96">
+        <v>195</v>
       </c>
       <c r="B96" s="2">
         <v>9</v>
@@ -1816,8 +1480,8 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" t="s">
-        <v>99</v>
+      <c r="A97">
+        <v>196</v>
       </c>
       <c r="B97" s="2">
         <v>9</v>
@@ -1827,8 +1491,8 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>100</v>
+      <c r="A98">
+        <v>197</v>
       </c>
       <c r="B98" s="2">
         <v>9</v>
@@ -1838,8 +1502,8 @@
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" t="s">
-        <v>101</v>
+      <c r="A99">
+        <v>198</v>
       </c>
       <c r="B99" s="2">
         <v>9</v>
@@ -1849,8 +1513,8 @@
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>102</v>
+      <c r="A100">
+        <v>199</v>
       </c>
       <c r="B100" s="2">
         <v>9</v>
@@ -1860,8 +1524,8 @@
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>103</v>
+      <c r="A101">
+        <v>200</v>
       </c>
       <c r="B101" s="2">
         <v>9</v>
@@ -1871,8 +1535,8 @@
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>104</v>
+      <c r="A102">
+        <v>201</v>
       </c>
       <c r="B102" s="2">
         <v>9</v>
@@ -1882,8 +1546,8 @@
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" t="s">
-        <v>105</v>
+      <c r="A103">
+        <v>202</v>
       </c>
       <c r="B103" s="2">
         <v>8</v>
@@ -1893,8 +1557,8 @@
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>106</v>
+      <c r="A104">
+        <v>203</v>
       </c>
       <c r="B104" s="2">
         <v>8</v>
@@ -1904,8 +1568,8 @@
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" t="s">
-        <v>107</v>
+      <c r="A105">
+        <v>204</v>
       </c>
       <c r="B105" s="2">
         <v>8</v>
@@ -1915,8 +1579,8 @@
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>108</v>
+      <c r="A106">
+        <v>205</v>
       </c>
       <c r="B106" s="2">
         <v>8</v>
@@ -1926,8 +1590,8 @@
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>109</v>
+      <c r="A107">
+        <v>206</v>
       </c>
       <c r="B107" s="2">
         <v>8</v>
@@ -1937,8 +1601,8 @@
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>110</v>
+      <c r="A108">
+        <v>207</v>
       </c>
       <c r="B108" s="2">
         <v>8</v>
@@ -1948,8 +1612,8 @@
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" t="s">
-        <v>111</v>
+      <c r="A109">
+        <v>208</v>
       </c>
       <c r="B109" s="2">
         <v>7</v>

</xml_diff>